<commit_message>
New items added and new status for the HTML report
</commit_message>
<xml_diff>
--- a/HTML_spectral_qc.xlsx
+++ b/HTML_spectral_qc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biqing/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3C5F4F6-E47E-EF43-8815-C7866114B5AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453ABF9E-C7F2-6144-9E18-D5EF4E1F1AC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="2500" windowWidth="28040" windowHeight="17440" xr2:uid="{02FCD511-79FF-2E40-8E14-DA3C6E4AF1D5}"/>
+    <workbookView xWindow="940" yWindow="1660" windowWidth="28040" windowHeight="17440" xr2:uid="{02FCD511-79FF-2E40-8E14-DA3C6E4AF1D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
   <si>
     <t>Suggested by</t>
   </si>
@@ -139,6 +139,18 @@
   </si>
   <si>
     <t>number_ant</t>
+  </si>
+  <si>
+    <t>Processed channel range</t>
+  </si>
+  <si>
+    <t>slurmOutput/&lt;latest_executed&gt;.sh</t>
+  </si>
+  <si>
+    <t>askapsoft</t>
+  </si>
+  <si>
+    <t>chan_range</t>
   </si>
 </sst>
 </file>
@@ -552,18 +564,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B70E992-8BAC-2A4B-A818-5F7A35BCEA59}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="29" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="56.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="46" style="2" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="57.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="46.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="29.1640625" style="2" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="2"/>
   </cols>
@@ -653,6 +665,9 @@
       <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
@@ -749,16 +764,22 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5"/>
       <c r="E14" s="2" t="s">
@@ -767,39 +788,39 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5"/>
       <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="E16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="E18" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="6"/>
       <c r="E19" s="2" t="s">
@@ -808,7 +829,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="6"/>
       <c r="E20" s="2" t="s">
@@ -817,10 +838,19 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="6"/>
       <c r="E21" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="E22" s="2" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest version with new parameters
Work in progress
</commit_message>
<xml_diff>
--- a/HTML_spectral_qc.xlsx
+++ b/HTML_spectral_qc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biqing/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A5F133-5078-954C-B284-5588F96B1FC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F5BF0B-5519-AA41-91BD-746C220B64C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="540" windowWidth="35820" windowHeight="17440" xr2:uid="{02FCD511-79FF-2E40-8E14-DA3C6E4AF1D5}"/>
+    <workbookView xWindow="2580" yWindow="540" windowWidth="35820" windowHeight="17440" xr2:uid="{02FCD511-79FF-2E40-8E14-DA3C6E4AF1D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="79">
   <si>
     <t>Status</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Currently using example file</t>
   </si>
   <si>
-    <t>Expected RMS</t>
-  </si>
-  <si>
     <t>theoretical_rms_mjy</t>
   </si>
   <si>
@@ -253,6 +250,18 @@
   </si>
   <si>
     <t>beamNoise_plots, beamMinMax_plots</t>
+  </si>
+  <si>
+    <t>Summary plot for MAD max flux density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summary plot for mean RMS </t>
+  </si>
+  <si>
+    <t>Not the best metric but can be compared to theoretical RMS</t>
+  </si>
+  <si>
+    <t>Theoretical RMS</t>
   </si>
 </sst>
 </file>
@@ -364,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -376,6 +385,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,15 +700,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B70E992-8BAC-2A4B-A818-5F7A35BCEA59}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="29"/>
   <cols>
-    <col min="1" max="1" width="56.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="64.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="86.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="61.1640625" style="2" customWidth="1"/>
@@ -1070,14 +1080,14 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>18</v>
@@ -1088,7 +1098,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>0</v>
@@ -1109,10 +1119,10 @@
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>18</v>
@@ -1124,10 +1134,10 @@
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>18</v>
@@ -1139,77 +1149,105 @@
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="B31" s="4"/>
+      <c r="C31" s="7"/>
+      <c r="E31" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="E32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="B33" s="11"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="B34" s="11"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D35" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E35" s="9" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="E34" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="E35" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B36" s="6"/>
+      <c r="C36" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E36" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B37" s="6"/>
       <c r="E37" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="E38" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="E39" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="E40" s="2" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated status and adding new parameters
</commit_message>
<xml_diff>
--- a/HTML_spectral_qc.xlsx
+++ b/HTML_spectral_qc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biqing/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F5BF0B-5519-AA41-91BD-746C220B64C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D605D2F2-07A2-744A-982E-46A368F01748}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="540" windowWidth="35820" windowHeight="17440" xr2:uid="{02FCD511-79FF-2E40-8E14-DA3C6E4AF1D5}"/>
+    <workbookView xWindow="3040" yWindow="1980" windowWidth="30780" windowHeight="16080" xr2:uid="{02FCD511-79FF-2E40-8E14-DA3C6E4AF1D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="95">
   <si>
     <t>Status</t>
   </si>
@@ -126,9 +126,6 @@
     <t>bmin</t>
   </si>
   <si>
-    <t xml:space="preserve">Max flux density </t>
-  </si>
-  <si>
     <t>Processed output directory/cubeStats*contsub.txt</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>Edited by</t>
   </si>
   <si>
-    <t>Unknown (fits header)</t>
-  </si>
-  <si>
     <t>Channel width</t>
   </si>
   <si>
@@ -153,9 +147,6 @@
     <t>metadata/mslist-scienceData*txt</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>metadata/mslist-&lt;date&gt;*txt</t>
   </si>
   <si>
@@ -262,13 +253,70 @@
   </si>
   <si>
     <t>Theoretical RMS</t>
+  </si>
+  <si>
+    <t>slurmOutput/&lt;latest&gt;.sh</t>
+  </si>
+  <si>
+    <t>List of bad channels</t>
+  </si>
+  <si>
+    <t>BAD_CHANS, QC_badchan_id</t>
+  </si>
+  <si>
+    <t>Figures/*png</t>
+  </si>
+  <si>
+    <t>Additional items</t>
+  </si>
+  <si>
+    <t>processed output directory/cubeStats*contsub.txt</t>
+  </si>
+  <si>
+    <t>processed output directory/image.restored.*contsub.fits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value needs checking </t>
+  </si>
+  <si>
+    <t>Might need 10MHz check, noise level is expected to change</t>
+  </si>
+  <si>
+    <t>Need to take into account flagged percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checking for the effects of sola intereference </t>
+  </si>
+  <si>
+    <t>List of HIPASS sources within 6x6 sq deg</t>
+  </si>
+  <si>
+    <t>Pull from vizier HICAT</t>
+  </si>
+  <si>
+    <t>hipass_cat</t>
+  </si>
+  <si>
+    <t>Doesn't work if it is diamond shape like the Eridanus field</t>
+  </si>
+  <si>
+    <t>mad_maxfdensity</t>
+  </si>
+  <si>
+    <t>Max flux density</t>
+  </si>
+  <si>
+    <t>beam_MADMFD_fig, MADMFD_plot</t>
+  </si>
+  <si>
+    <t>beam_Avg_RMS_fig, AvgRMS_plot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -325,8 +373,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,6 +398,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -386,6 +448,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B70E992-8BAC-2A4B-A818-5F7A35BCEA59}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="29"/>
@@ -713,7 +778,7 @@
     <col min="3" max="3" width="86.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="61.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="29.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18" style="2" customWidth="1"/>
+    <col min="6" max="6" width="44.1640625" style="2" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -731,10 +796,10 @@
         <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -758,10 +823,10 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>18</v>
@@ -773,7 +838,7 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>21</v>
@@ -788,7 +853,7 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>22</v>
@@ -803,25 +868,25 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>30</v>
@@ -836,7 +901,7 @@
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>24</v>
@@ -851,7 +916,7 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>25</v>
@@ -866,7 +931,7 @@
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>26</v>
@@ -881,7 +946,7 @@
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>27</v>
@@ -896,7 +961,7 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>28</v>
@@ -905,19 +970,19 @@
         <v>18</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>18</v>
@@ -925,14 +990,14 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="2" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>18</v>
@@ -942,9 +1007,9 @@
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="4"/>
       <c r="C15" s="2" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>31</v>
@@ -957,9 +1022,9 @@
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="2" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>32</v>
@@ -970,7 +1035,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>0</v>
@@ -982,19 +1047,19 @@
         <v>20</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>18</v>
@@ -1002,14 +1067,14 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>18</v>
@@ -1017,14 +1082,14 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>18</v>
@@ -1032,32 +1097,32 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>18</v>
@@ -1065,79 +1130,85 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="E24" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="B26" s="3"/>
+      <c r="E26" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="12"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D28" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>18</v>
+      <c r="E28" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>18</v>
@@ -1145,14 +1216,14 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>18</v>
@@ -1160,95 +1231,159 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="B31" s="4"/>
-      <c r="C31" s="7"/>
+      <c r="C31" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="E31" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B32" s="4"/>
+      <c r="C32" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="E32" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="B33" s="11"/>
-    </row>
-    <row r="34" spans="1:5">
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="B34" s="11"/>
     </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:6">
+      <c r="B35" s="11"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D36" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="2" t="s">
+      <c r="E36" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="2" t="s">
+      <c r="D37" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="E37" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="B38" s="6"/>
       <c r="E38" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B39" s="6"/>
       <c r="E39" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:6">
       <c r="A40" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B40" s="6"/>
       <c r="E40" s="2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="E41" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>